<commit_message>
Update : Environment & Mobile Setting
</commit_message>
<xml_diff>
--- a/Assets/_Project/Scripts/StageDB/StageDB.xlsx
+++ b/Assets/_Project/Scripts/StageDB/StageDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han\Desktop\Unity Projects\TakeBackMyHome\Assets\_Project\Scripts\StageDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A171D8C-F578-4058-B9FC-35CF5C14074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FFCBF4-3279-47C1-96AD-8CF577093E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F7E96E5E-2B56-429B-B6A1-4F9E1CD4EB8E}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -490,10 +490,10 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="F8">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -610,7 +610,7 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -815,10 +815,10 @@
         <v>2</v>
       </c>
       <c r="E20">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F20">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -915,10 +915,10 @@
         <v>2</v>
       </c>
       <c r="E25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -935,10 +935,10 @@
         <v>2</v>
       </c>
       <c r="E26">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1140,10 +1140,10 @@
         <v>2</v>
       </c>
       <c r="E37">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F37">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1240,10 +1240,10 @@
         <v>2</v>
       </c>
       <c r="E42">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F42">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1260,10 +1260,10 @@
         <v>2</v>
       </c>
       <c r="E43">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="F43">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1465,10 +1465,10 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F54">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1568,7 +1568,7 @@
         <v>10</v>
       </c>
       <c r="F59">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1585,10 +1585,10 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F60">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1790,10 +1790,10 @@
         <v>2</v>
       </c>
       <c r="E71">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F71">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -1893,7 +1893,7 @@
         <v>10</v>
       </c>
       <c r="F76">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -1910,10 +1910,10 @@
         <v>2</v>
       </c>
       <c r="E77">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F77">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update : UI Setting & StageScene
</commit_message>
<xml_diff>
--- a/Assets/_Project/Scripts/StageDB/StageDB.xlsx
+++ b/Assets/_Project/Scripts/StageDB/StageDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han\Desktop\Unity Projects\TakeBackMyHome\Assets\_Project\Scripts\StageDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D9B93F-25E2-4A38-955C-1BF0F1A65F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DC5081-45F8-48F0-ADA2-0C4E12CE81FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F7E96E5E-2B56-429B-B6A1-4F9E1CD4EB8E}"/>
   </bookViews>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73F9436-191E-42A0-8B94-82AD64CF8B86}">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="U71" sqref="U71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -1124,7 +1124,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
@@ -1454,7 +1454,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C52" s="1">
         <v>0</v>
@@ -1784,7 +1784,7 @@
         <v>4</v>
       </c>
       <c r="B69" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C69" s="1">
         <v>5</v>
@@ -2114,7 +2114,7 @@
         <v>5</v>
       </c>
       <c r="B86" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C86" s="1">
         <v>5</v>

</xml_diff>